<commit_message>
Add fixed; begin with clustering conventionals for investment modelling
</commit_message>
<xml_diff>
--- a/raw_data_input/powerplants_public/Liste_Zuschlaege_April2021.xlsx
+++ b/raw_data_input/powerplants_public/Liste_Zuschlaege_April2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\POMMES_public\pommes-data\raw_data_input\powerplants_public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F949FD-CD14-4A7B-81DD-B9ED3DABE074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D40EA2-A54D-4D15-9CD7-04322CF93C60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32370" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Name des Bieters</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>BNA1097</t>
+  </si>
+  <si>
+    <t>BNA0662b</t>
+  </si>
+  <si>
+    <t>BNA0331</t>
   </si>
 </sst>
 </file>
@@ -844,10 +850,10 @@
   <dimension ref="A4:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,6 +1096,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
       <c r="B19" s="12" t="s">
         <v>26</v>
       </c>
@@ -1108,6 +1117,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
       <c r="B20" s="16" t="s">
         <v>5</v>
       </c>
@@ -1142,21 +1154,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Aktenrelevant xmlns="03bcae2d-d3c0-4e5e-8622-15c96813d07f" xsi:nil="true"/>
+    <Kommentar xmlns="03bcae2d-d3c0-4e5e-8622-15c96813d07f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Aktenrelevant xmlns="03bcae2d-d3c0-4e5e-8622-15c96813d07f" xsi:nil="true"/>
-    <Kommentar xmlns="03bcae2d-d3c0-4e5e-8622-15c96813d07f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1297,14 +1309,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05A41544-B0F9-44F6-8E00-5F4E73CF55F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0908DF05-E6A7-4568-9CB8-5BAB985E9308}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1316,6 +1320,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05A41544-B0F9-44F6-8E00-5F4E73CF55F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>